<commit_message>
Considering Dinic's Algorithm for testing as well
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\Maximum-Flow-Algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8ED2DC-02F0-4BB8-AA3B-C344DCDCC51C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067959E3-AB62-4167-A457-652CC00B24FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{C8CBCAC3-70B2-44D4-A8A3-2DDD91A98114}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Maximum Flow Algorithm {Ford-Fulkerson}</t>
   </si>
@@ -116,12 +116,45 @@
   <si>
     <t>ladder_7</t>
   </si>
+  <si>
+    <t>Ladder</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Bridge</t>
+  </si>
+  <si>
+    <t>m  = b =</t>
+  </si>
+  <si>
+    <t>c =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a = </t>
+  </si>
+  <si>
+    <t>T(N)</t>
+  </si>
+  <si>
+    <t>~1</t>
+  </si>
+  <si>
+    <t>~3</t>
+  </si>
+  <si>
+    <t>T(N) = N^3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +190,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -307,6 +355,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -315,8 +372,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0094C8"/>
       <color rgb="FF4FD1FF"/>
-      <color rgb="FF0094C8"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2553,16 +2610,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>301664</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>447021</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>80492</xdr:rowOff>
+      <xdr:rowOff>239485</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>277906</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>62753</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>423903</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>12357</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2589,16 +2646,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>565933</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>322757</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>169564</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>38073</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>47327</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>208311</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>87668</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2923,10 +2980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D240016B-EC40-46A3-93C6-B57F047E01EF}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE11" sqref="AE11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2936,9 +2993,11 @@
     <col min="4" max="8" width="12.5546875" customWidth="1"/>
     <col min="9" max="9" width="14.88671875" customWidth="1"/>
     <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="17" max="17" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2952,7 +3011,7 @@
       <c r="I1" s="15"/>
       <c r="J1" s="16"/>
     </row>
-    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -2982,7 +3041,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="12" t="s">
         <v>7</v>
@@ -2998,7 +3057,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" ht="18" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -3031,8 +3090,16 @@
         <f>(I4/1000000000)</f>
         <v>7.6959999999999995E-4</v>
       </c>
+      <c r="M4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="17"/>
+      <c r="T4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="U4" s="17"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -3065,8 +3132,34 @@
         <f>(I5/1000000000)</f>
         <v>6.8156E-4</v>
       </c>
+      <c r="M5" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5">
+        <f>(N14-N13)/(M14-M13)</f>
+        <v>0.72100944282412915</v>
+      </c>
+      <c r="T5" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="U5" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="W5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X5">
+        <f>(U13-U14)/(T13-T14)</f>
+        <v>2.6926325363037655</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -3099,8 +3192,30 @@
         <f t="shared" ref="J6:J10" si="1">(I6/1000000000)</f>
         <v>9.4169999999999996E-4</v>
       </c>
+      <c r="M6" s="4">
+        <f>LOG(B4,2)</f>
+        <v>2.5849625007211561</v>
+      </c>
+      <c r="N6" s="4">
+        <f>LOG(D4,2)</f>
+        <v>19.675385099561947</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T6" s="4">
+        <f>LOG(B14,2)</f>
+        <v>2.5849625007211561</v>
+      </c>
+      <c r="U6" s="4">
+        <f>LOG(D14,2)</f>
+        <v>20.553093012995632</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -3133,8 +3248,24 @@
         <f t="shared" si="1"/>
         <v>1.10406E-3</v>
       </c>
+      <c r="M7" s="4">
+        <f t="shared" ref="M7:M14" si="2">LOG(B5,2)</f>
+        <v>3.3219280948873626</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" ref="N7:N14" si="3">LOG(D5,2)</f>
+        <v>19.323556195543976</v>
+      </c>
+      <c r="T7" s="4">
+        <f>LOG(B15,2)</f>
+        <v>3.5849625007211565</v>
+      </c>
+      <c r="U7" s="4">
+        <f>LOG(D15,2)</f>
+        <v>19.586005943326022</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -3167,8 +3298,38 @@
         <f t="shared" si="1"/>
         <v>1.3472200000000001E-3</v>
       </c>
+      <c r="M8" s="4">
+        <f t="shared" si="2"/>
+        <v>4.1699250014423122</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="3"/>
+        <v>20.70125569054721</v>
+      </c>
+      <c r="P8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8">
+        <f>(N14-(Q5*M14))</f>
+        <v>16.943569678874894</v>
+      </c>
+      <c r="T8" s="4">
+        <f>LOG(B16,2)</f>
+        <v>4.584962500721157</v>
+      </c>
+      <c r="U8" s="4">
+        <f>LOG(D16,2)</f>
+        <v>20.235495405804869</v>
+      </c>
+      <c r="W8" t="s">
+        <v>35</v>
+      </c>
+      <c r="X8">
+        <f>(U14-(X5*T14))</f>
+        <v>1.7905269800426709</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
@@ -3201,8 +3362,38 @@
         <f t="shared" si="1"/>
         <v>2.46488E-3</v>
       </c>
+      <c r="M9" s="4">
+        <f t="shared" si="2"/>
+        <v>5.08746284125034</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="3"/>
+        <v>20.756865754721026</v>
+      </c>
+      <c r="P9" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q9">
+        <f>POWER(2, Q8)</f>
+        <v>126044.15380007106</v>
+      </c>
+      <c r="T9" s="4">
+        <f>LOG(B17,2)</f>
+        <v>5.584962500721157</v>
+      </c>
+      <c r="U9" s="4">
+        <f>LOG(D17,2)</f>
+        <v>21.130439848841995</v>
+      </c>
+      <c r="W9" t="s">
+        <v>36</v>
+      </c>
+      <c r="X9">
+        <f>POWER(2, X8)</f>
+        <v>3.4594123303800921</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -3235,8 +3426,24 @@
         <f t="shared" si="1"/>
         <v>7.4446E-3</v>
       </c>
+      <c r="M10" s="4">
+        <f t="shared" si="2"/>
+        <v>6.0443941193584534</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" si="3"/>
+        <v>20.653247454533645</v>
+      </c>
+      <c r="T10" s="4">
+        <f>LOG(B18,2)</f>
+        <v>6.5849625007211561</v>
+      </c>
+      <c r="U10" s="4">
+        <f>LOG(D18,2)</f>
+        <v>22.183317954421362</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -3269,8 +3476,24 @@
         <f>(I11/1000000000)</f>
         <v>1.26112802E-2</v>
       </c>
+      <c r="M11" s="4">
+        <f t="shared" si="2"/>
+        <v>7.0223678130284544</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" si="3"/>
+        <v>21.844869703287102</v>
+      </c>
+      <c r="T11" s="4">
+        <f>LOG(B19,2)</f>
+        <v>7.5849625007211561</v>
+      </c>
+      <c r="U11" s="4">
+        <f>LOG(D19,2)</f>
+        <v>24.148558816331704</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -3303,8 +3526,24 @@
         <f>(I12/1000000000)</f>
         <v>2.1809119600000003E-2</v>
       </c>
+      <c r="M12" s="4">
+        <f t="shared" si="2"/>
+        <v>8.011227255423254</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="3"/>
+        <v>22.579205432808724</v>
+      </c>
+      <c r="T12" s="4">
+        <f>LOG(B20,2)</f>
+        <v>8.5849625007211561</v>
+      </c>
+      <c r="U12" s="4">
+        <f>LOG(D20,2)</f>
+        <v>25.396011397614618</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -3315,8 +3554,27 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
+      <c r="M13" s="4">
+        <f t="shared" si="2"/>
+        <v>9.0056245491938789</v>
+      </c>
+      <c r="N13" s="4">
+        <f t="shared" si="3"/>
+        <v>23.436710017372473</v>
+      </c>
+      <c r="P13" t="s">
+        <v>37</v>
+      </c>
+      <c r="T13" s="4">
+        <f>LOG(B21,2)</f>
+        <v>9.5849625007211561</v>
+      </c>
+      <c r="U13" s="4">
+        <f>LOG(D21,2)</f>
+        <v>27.59930886873596</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -3349,8 +3607,24 @@
         <f>(I14/1000000000)</f>
         <v>1.0839998E-3</v>
       </c>
+      <c r="M14" s="4">
+        <f t="shared" si="2"/>
+        <v>10.002815015607053</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" si="3"/>
+        <v>24.155693759950569</v>
+      </c>
+      <c r="T14" s="4">
+        <f>LOG(B22,2)</f>
+        <v>10.584962500721156</v>
+      </c>
+      <c r="U14" s="4">
+        <f>LOG(D22,2)</f>
+        <v>30.291941405039726</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -3384,7 +3658,7 @@
         <v>8.1836039999999999E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
@@ -3410,15 +3684,15 @@
         <v>1554600</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" ref="I16:I20" si="2">AVERAGE(D16:H16)</f>
+        <f t="shared" ref="I16:I20" si="4">AVERAGE(D16:H16)</f>
         <v>1660800</v>
       </c>
       <c r="J16" s="4">
-        <f t="shared" ref="J16:J20" si="3">(I16/1000000000)</f>
+        <f t="shared" ref="J16:J20" si="5">(I16/1000000000)</f>
         <v>1.6608E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
@@ -3444,15 +3718,18 @@
         <v>2349500</v>
       </c>
       <c r="I17" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2196340</v>
       </c>
       <c r="J17" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.1963400000000002E-3</v>
       </c>
+      <c r="X17" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
@@ -3478,15 +3755,15 @@
         <v>6591100</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5797060</v>
       </c>
       <c r="J18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.7970599999999997E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
@@ -3512,15 +3789,15 @@
         <v>22709500</v>
       </c>
       <c r="I19" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>23391860</v>
       </c>
       <c r="J19" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.339186E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
@@ -3546,15 +3823,15 @@
         <v>41959100</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>42419080</v>
       </c>
       <c r="J20" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.2419079999999998E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
@@ -3588,7 +3865,7 @@
         <v>0.25327526039999998</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
@@ -3622,24 +3899,24 @@
         <v>1.6202573192</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="1">
         <v>1945930800</v>
@@ -3652,14 +3929,20 @@
         <v>1924121680.4000001</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="1"/>
+    <row r="29" spans="1:24" ht="18" x14ac:dyDescent="0.3">
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="A1:J1"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3726,6 +4009,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005C324ADAAA76C24086318E2213935189" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="98480c2a5ea3f6971cee195b33bf0533">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e555b152-19e3-4faf-a022-c0cb6a9a7abe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0af9b9821d5e6fa0efb2df04688a4f72" ns3:_="">
     <xsd:import namespace="e555b152-19e3-4faf-a022-c0cb6a9a7abe"/>
@@ -3871,22 +4169,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B20362A-FBE8-4BCF-AD59-EC7D77F3AE43}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e555b152-19e3-4faf-a022-c0cb6a9a7abe"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04C8B86E-EE2A-4BE3-BE59-C4547F14ECA3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F8AFD12-5C06-45D0-8D29-40BC29B69E4C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3902,28 +4209,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04C8B86E-EE2A-4BE3-BE59-C4547F14ECA3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B20362A-FBE8-4BCF-AD59-EC7D77F3AE43}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e555b152-19e3-4faf-a022-c0cb6a9a7abe"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added some new max flow implementations, for further testing and analysis
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\Maximum-Flow-Algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067959E3-AB62-4167-A457-652CC00B24FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D745F6F2-BE2C-4B5F-8223-50A6CCB72E8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{C8CBCAC3-70B2-44D4-A8A3-2DDD91A98114}"/>
   </bookViews>
@@ -579,13 +579,13 @@
                   <c:v>769600</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>681560</c:v>
+                  <c:v>839000</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>941700</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1104060</c:v>
+                  <c:v>1120580</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1347220</c:v>
@@ -594,7 +594,7 @@
                   <c:v>2464880</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7444600</c:v>
+                  <c:v>6881680</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>12611280.199999999</c:v>
@@ -1129,7 +1129,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1083999.8</c:v>
+                  <c:v>805020</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>818360.4</c:v>
@@ -2610,16 +2610,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>447021</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>239485</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>131336</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>87085</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>423903</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>12357</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>347704</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>88557</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2646,16 +2646,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>322757</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>169564</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>311871</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>115136</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>208311</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>87668</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>872340</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>33239</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2982,8 +2982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D240016B-EC40-46A3-93C6-B57F047E01EF}">
   <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3110,27 +3110,27 @@
         <v>17</v>
       </c>
       <c r="D5" s="4">
-        <v>656100</v>
+        <v>918400</v>
       </c>
       <c r="E5" s="4">
-        <v>644500</v>
+        <v>827700</v>
       </c>
       <c r="F5" s="4">
-        <v>779400</v>
+        <v>826900</v>
       </c>
       <c r="G5" s="4">
-        <v>532700</v>
+        <v>826900</v>
       </c>
       <c r="H5" s="4">
         <v>795100</v>
       </c>
       <c r="I5" s="4">
         <f>AVERAGE(D5:H5)</f>
-        <v>681560</v>
+        <v>839000</v>
       </c>
       <c r="J5" s="4">
         <f>(I5/1000000000)</f>
-        <v>6.8156E-4</v>
+        <v>8.3900000000000001E-4</v>
       </c>
       <c r="M5" s="19" t="s">
         <v>31</v>
@@ -3209,7 +3209,7 @@
       </c>
       <c r="U6" s="4">
         <f>LOG(D14,2)</f>
-        <v>20.553093012995632</v>
+        <v>19.521332056309152</v>
       </c>
       <c r="X6" s="2" t="s">
         <v>39</v>
@@ -3229,7 +3229,7 @@
         <v>1771900</v>
       </c>
       <c r="E7" s="4">
-        <v>1018500</v>
+        <v>910700</v>
       </c>
       <c r="F7" s="4">
         <v>946000</v>
@@ -3238,15 +3238,15 @@
         <v>963300</v>
       </c>
       <c r="H7" s="4">
-        <v>820600</v>
+        <v>1011000</v>
       </c>
       <c r="I7" s="4">
         <f t="shared" si="0"/>
-        <v>1104060</v>
+        <v>1120580</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="1"/>
-        <v>1.10406E-3</v>
+        <v>1.1205799999999999E-3</v>
       </c>
       <c r="M7" s="4">
         <f t="shared" ref="M7:M14" si="2">LOG(B5,2)</f>
@@ -3254,7 +3254,7 @@
       </c>
       <c r="N7" s="4">
         <f t="shared" ref="N7:N14" si="3">LOG(D5,2)</f>
-        <v>19.323556195543976</v>
+        <v>19.808763116450415</v>
       </c>
       <c r="T7" s="4">
         <f>LOG(B15,2)</f>
@@ -3407,7 +3407,7 @@
         <v>6266400</v>
       </c>
       <c r="E10" s="4">
-        <v>9301300</v>
+        <v>6486700</v>
       </c>
       <c r="F10" s="4">
         <v>5689000</v>
@@ -3420,11 +3420,11 @@
       </c>
       <c r="I10" s="4">
         <f t="shared" si="0"/>
-        <v>7444600</v>
+        <v>6881680</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="1"/>
-        <v>7.4446E-3</v>
+        <v>6.8816800000000003E-3</v>
       </c>
       <c r="M10" s="4">
         <f t="shared" si="2"/>
@@ -3585,27 +3585,27 @@
         <v>9</v>
       </c>
       <c r="D14" s="4">
-        <v>1538500</v>
+        <v>752500</v>
       </c>
       <c r="E14" s="4">
-        <v>954699</v>
+        <v>688000</v>
       </c>
       <c r="F14" s="4">
-        <v>873100</v>
+        <v>717900</v>
       </c>
       <c r="G14" s="4">
-        <v>961600</v>
+        <v>774600</v>
       </c>
       <c r="H14" s="4">
         <v>1092100</v>
       </c>
       <c r="I14" s="4">
         <f>AVERAGE(D14:H14)</f>
-        <v>1083999.8</v>
+        <v>805020</v>
       </c>
       <c r="J14" s="4">
         <f>(I14/1000000000)</f>
-        <v>1.0839998E-3</v>
+        <v>8.0502000000000004E-4</v>
       </c>
       <c r="M14" s="4">
         <f t="shared" si="2"/>

</xml_diff>